<commit_message>
export the event, correctly export the city
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/records/exportRecords.xlsx
+++ b/owlcms/src/main/resources/templates/records/exportRecords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B367115-C037-4A1F-95CA-6D3B1ECA6F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B886DF5F-9FF8-4E0F-A4AA-603FA2B7FC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="3135" windowWidth="23940" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewRecords" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Lift</t>
   </si>
@@ -209,9 +209,6 @@
     <t>${r.recordDateAsString}</t>
   </si>
   <si>
-    <t>${competition.competitionCity}</t>
-  </si>
-  <si>
     <t>${r.groupNameString}</t>
   </si>
   <si>
@@ -219,6 +216,15 @@
   </si>
   <si>
     <t>M/F</t>
+  </si>
+  <si>
+    <t>${r.eventLocation}</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>${r.event}</t>
   </si>
 </sst>
 </file>
@@ -687,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>10</v>
@@ -761,7 +767,9 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -803,7 +811,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>22</v>
@@ -824,12 +832,14 @@
         <v>29</v>
       </c>
       <c r="O3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="9"/>
+      <c r="Q3" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1288,7 +1298,7 @@
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:F1048576" xr:uid="{A2E907D7-3179-4C92-B9E8-43D2D96CBEC9}">
       <formula1>0</formula1>
       <formula2>120</formula2>
@@ -1301,21 +1311,12 @@
       <formula1>0</formula1>
       <formula2>300</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4" xr:uid="{DD6A1ACE-E119-406B-B54E-8F08A2EE531D}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD6A1ACE-E119-406B-B54E-8F08A2EE531D}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2 D4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added processing of event at which record was broken.
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/records/exportRecords.xlsx
+++ b/owlcms/src/main/resources/templates/records/exportRecords.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B886DF5F-9FF8-4E0F-A4AA-603FA2B7FC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B4EEE5-8F32-4B34-9F84-D290CF8CAC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3135" windowWidth="23940" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NewRecords" sheetId="1" r:id="rId1"/>
+    <sheet name="Records" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -694,7 +694,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
export and report current records; closes #1136
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/records/exportRecords.xlsx
+++ b/owlcms/src/main/resources/templates/records/exportRecords.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B4EEE5-8F32-4B34-9F84-D290CF8CAC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF037DD-672F-45D1-9E74-0A54AFC571C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -693,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1009,6 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -1023,7 +1024,6 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1039,7 +1039,6 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1055,7 +1054,6 @@
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1071,7 +1069,6 @@
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -1087,7 +1084,6 @@
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -1103,7 +1099,6 @@
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -1119,7 +1114,6 @@
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -1135,7 +1129,6 @@
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -1151,7 +1144,6 @@
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1167,7 +1159,6 @@
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1183,7 +1174,6 @@
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1199,7 +1189,6 @@
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -1215,7 +1204,6 @@
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1231,7 +1219,6 @@
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -1247,7 +1234,6 @@
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1263,7 +1249,6 @@
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>

</xml_diff>